<commit_message>
- Refactory dos arquivos e adição do arguments.py
</commit_message>
<xml_diff>
--- a/file/sample.xlsx
+++ b/file/sample.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -366,7 +366,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="n">
-        <v>42808.43560755787</v>
+        <v>42916.68403201389</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>

</xml_diff>